<commit_message>
Finalizing Phase 2 Documents
Design Document - removed some images and rewrote references
Design Presentation - Fixed spelling issues and moving around slides
Gantt Chart - Updated to work done up to 4/10 with the completion of the document
</commit_message>
<xml_diff>
--- a/Phase 2 Documents/Gantt Chart - Updated P2.xlsx
+++ b/Phase 2 Documents/Gantt Chart - Updated P2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\communicationsGroup4\Phase 2 Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lupo/Documents/GitHub/communicationsGroup4/Phase 2 Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136E0AB5-964A-4932-8FFD-922AB555308B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8A913F-1AF5-CA46-A21F-C579A57075B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
   <si>
     <t>Development</t>
   </si>
@@ -190,22 +190,22 @@
     <t>Talhah/Zoheb</t>
   </si>
   <si>
-    <t>1. Class Diagram Updated</t>
-  </si>
-  <si>
-    <t>2. Classes Descriptions</t>
-  </si>
-  <si>
-    <t>3. Sequence Diagrams</t>
-  </si>
-  <si>
-    <t>4. Prototype</t>
-  </si>
-  <si>
     <t>4/10 (Thursday)</t>
   </si>
   <si>
     <t>1. Use Case Diagram/ Cases</t>
+  </si>
+  <si>
+    <t>2. Updated Class Diagram</t>
+  </si>
+  <si>
+    <t>3. Classes Descriptions</t>
+  </si>
+  <si>
+    <t>4. Sequence Diagrams</t>
+  </si>
+  <si>
+    <t>5. Prototype</t>
   </si>
 </sst>
 </file>
@@ -241,13 +241,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -276,8 +269,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,18 +286,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
-        <bgColor rgb="FFF4CCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -501,14 +490,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -537,23 +525,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -562,7 +547,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -571,31 +556,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Accent2" xfId="3" builtinId="33"/>
-    <cellStyle name="Accent4" xfId="4" builtinId="41"/>
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="4">
+    <cellStyle name="Accent2" xfId="2" builtinId="33"/>
+    <cellStyle name="Accent4" xfId="3" builtinId="41"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -876,62 +860,62 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="15" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:14" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
@@ -971,651 +955,367 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="20"/>
-    </row>
-    <row r="4" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N3" s="19"/>
+    </row>
+    <row r="4" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23" t="s">
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="25"/>
-    </row>
-    <row r="5" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N4" s="23"/>
+    </row>
+    <row r="5" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="25"/>
-    </row>
-    <row r="6" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="N5" s="23"/>
+    </row>
+    <row r="6" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="25"/>
-    </row>
-    <row r="7" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="N6" s="23"/>
+    </row>
+    <row r="7" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="25"/>
-    </row>
-    <row r="8" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="N7" s="23"/>
+    </row>
+    <row r="8" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="25"/>
-    </row>
-    <row r="9" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="N8" s="23"/>
+    </row>
+    <row r="9" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="25"/>
-    </row>
-    <row r="10" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="25"/>
-    </row>
-    <row r="11" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="N10" s="23"/>
+    </row>
+    <row r="11" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="25"/>
-    </row>
-    <row r="12" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="N11" s="23"/>
+    </row>
+    <row r="12" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="25"/>
-    </row>
-    <row r="13" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="N12" s="23"/>
+    </row>
+    <row r="13" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="25"/>
-    </row>
-    <row r="14" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="24"/>
+      <c r="N13" s="23"/>
+    </row>
+    <row r="14" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="25"/>
-    </row>
-    <row r="15" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N14" s="23"/>
+    </row>
+    <row r="15" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="5"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="25"/>
-    </row>
-    <row r="16" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N15" s="23"/>
+    </row>
+    <row r="16" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="25"/>
-    </row>
-    <row r="17" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N16" s="23"/>
+    </row>
+    <row r="17" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="25"/>
-    </row>
-    <row r="18" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="N17" s="23"/>
+    </row>
+    <row r="18" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="25"/>
-    </row>
-    <row r="19" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
-        <v>56</v>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="26"/>
+      <c r="N18" s="23"/>
+    </row>
+    <row r="19" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="A19" s="27" t="s">
+        <v>58</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="25"/>
-    </row>
-    <row r="20" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
-        <v>57</v>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="N19" s="23"/>
+    </row>
+    <row r="20" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="A20" s="27" t="s">
+        <v>59</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="25"/>
-    </row>
-    <row r="21" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="25"/>
-    </row>
-    <row r="22" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="N20" s="23"/>
+    </row>
+    <row r="21" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="A21" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="N21" s="23"/>
+    </row>
+    <row r="22" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B22" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="25"/>
-    </row>
-    <row r="23" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="N22" s="23"/>
+    </row>
+    <row r="23" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="25"/>
-    </row>
-    <row r="24" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="25"/>
-    </row>
-    <row r="25" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="N23" s="23"/>
+    </row>
+    <row r="24" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="A24" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="N24" s="23"/>
+    </row>
+    <row r="25" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B25" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="25"/>
-    </row>
-    <row r="26" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="N25" s="23"/>
+    </row>
+    <row r="26" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B26" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="25"/>
-    </row>
-    <row r="27" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="N26" s="23"/>
+    </row>
+    <row r="27" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="25"/>
-    </row>
-    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="N27" s="23"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="25"/>
-    </row>
-    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J28" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="N28" s="23"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="25"/>
-    </row>
-    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N29" s="23"/>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="25"/>
-    </row>
-    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="25"/>
+      <c r="N30" s="23"/>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
-      <c r="N31" s="25"/>
-    </row>
-    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="23"/>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="25"/>
-    </row>
-    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="23"/>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="5"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="24"/>
-      <c r="N33" s="25"/>
-    </row>
-    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N33" s="23"/>
+    </row>
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="27"/>
-      <c r="N34" s="25"/>
-    </row>
-    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M34" s="25"/>
+      <c r="N34" s="23"/>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="24"/>
-      <c r="M35" s="24"/>
-      <c r="N35" s="27"/>
-    </row>
-    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="24"/>
-      <c r="L36" s="24"/>
-      <c r="M36" s="24"/>
-      <c r="N36" s="25"/>
-    </row>
-    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="24"/>
-      <c r="L37" s="24"/>
-      <c r="M37" s="24"/>
-      <c r="N37" s="25"/>
-    </row>
-    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24"/>
-      <c r="K38" s="24"/>
-      <c r="L38" s="24"/>
-      <c r="M38" s="24"/>
-      <c r="N38" s="25"/>
-    </row>
-    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N35" s="25"/>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N36" s="23"/>
+    </row>
+    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N37" s="23"/>
+    </row>
+    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N38" s="23"/>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="8"/>
-      <c r="N39" s="21"/>
+      <c r="N39" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>